<commit_message>
Updated sprint 3 execution and burndown chart
</commit_message>
<xml_diff>
--- a/sprint_backlog/sprint3/plan.xlsx
+++ b/sprint_backlog/sprint3/plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ajg\Documents (D)\Repositories\CSCC01\Team5\sprint_backlog\sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5190BF47-7F17-4092-8B12-187B7F0ADFBA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35654EE2-2D26-4B32-B5B6-854AB193BDAB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <r>
       <rPr>
@@ -300,6 +300,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -314,21 +329,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -715,7 +715,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,33 +730,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -791,7 +791,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -817,7 +817,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -841,7 +841,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
@@ -871,7 +871,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -899,7 +899,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
@@ -917,7 +917,7 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -940,10 +940,12 @@
       <c r="I9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -973,7 +975,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="3" t="s">
         <v>25</v>
       </c>
@@ -991,56 +993,56 @@
       <c r="J11" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>